<commit_message>
Heavily modified my python scraps directory
</commit_message>
<xml_diff>
--- a/csv2sql/Data/Test_Data_McMurdo.xlsx
+++ b/csv2sql/Data/Test_Data_McMurdo.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10713"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dsbrown/Prog/python/csv2sql/Data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F586D49-FC74-2941-87A4-BC661FF0A185}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14440" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test_Data_McMurdo.csv" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -297,7 +303,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -363,6 +369,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -687,14 +701,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BX2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="BU1" workbookViewId="0">
       <selection activeCell="BU1" sqref="BU1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
@@ -739,7 +753,7 @@
     <col min="76" max="76" width="37.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:76">
+    <row r="1" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -969,7 +983,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:76">
+    <row r="2" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>76</v>
       </c>

</xml_diff>